<commit_message>
Updated excel files after running the code with the changes
</commit_message>
<xml_diff>
--- a/data/interim/Impacts_per_ingredients.xlsx
+++ b/data/interim/Impacts_per_ingredients.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,72 +441,72 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Land Use (m2) Arable</t>
+          <t>Land Use Arable</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Land Use (m2) Fallow</t>
+          <t>Land Use Fallow</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Land Use (m2) Perm Past</t>
+          <t>Land Use Perm Past</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>GHG (kg CO2eq, IPCC 2013) LUC</t>
+          <t>GHG LUC</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>GHG (kg CO2eq, IPCC 2013) Feed</t>
+          <t>GHG Feed</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>GHG (kg CO2eq, IPCC 2013) Farm</t>
+          <t>GHG Farm</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>GHG (kg CO2eq, IPCC 2013) Processing</t>
+          <t>GHG Processing</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>GHG (kg CO2eq, IPCC 2013) Transport</t>
+          <t>GHG Transport</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>GHG (kg CO2eq, IPCC 2013) Packging</t>
+          <t>GHG Packging</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>GHG (kg CO2eq, IPCC 2013) Retail</t>
+          <t>GHG Retail</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Acid.(kg SO2eq)</t>
+          <t>Acidification</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Eutr. (kg PO43-eq)</t>
+          <t>Eutrophication</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Freshwater (L)</t>
+          <t>Freshwater Withdrawals (FW)</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Str-Wt WU (L eq)</t>
+          <t>Scarcity-Weighted FW</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
@@ -565,7 +565,7 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Recipe 1</t>
+          <t>Rice and Beef</t>
         </is>
       </c>
     </row>
@@ -619,385 +619,223 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Recipe 1</t>
+          <t>Rice and Beef</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9.749285</v>
+        <v>0.4186</v>
       </c>
       <c r="C4" t="n">
-        <v>2.367085</v>
+        <v>0.0616</v>
       </c>
       <c r="D4" t="n">
-        <v>76.48186</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>7.402089999999999</v>
+        <v>-0.004399999999999999</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8544899999999999</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>18.63214</v>
+        <v>0.7106</v>
       </c>
       <c r="H4" t="n">
-        <v>0.590395</v>
+        <v>0.013</v>
       </c>
       <c r="I4" t="n">
-        <v>0.17663</v>
+        <v>0.0192</v>
       </c>
       <c r="J4" t="n">
-        <v>0.129185</v>
+        <v>0.0168</v>
       </c>
       <c r="K4" t="n">
-        <v>0.08722000000000001</v>
+        <v>0.0126</v>
       </c>
       <c r="L4" t="n">
-        <v>0.09084095</v>
+        <v>0.004714</v>
       </c>
       <c r="M4" t="n">
-        <v>0.08669285</v>
+        <v>0.005944</v>
       </c>
       <c r="N4" t="n">
-        <v>788.7049999999999</v>
+        <v>392.4</v>
       </c>
       <c r="O4" t="n">
-        <v>18284.165</v>
+        <v>8655</v>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Recipe 1</t>
+          <t>Rice and chicken</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Rice</t>
+          <t>Chicken</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.4186</v>
+        <v>2.5753</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0616</v>
+        <v>0.83265</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.004399999999999999</v>
+        <v>1.1557</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
+        <v>0.807625</v>
       </c>
       <c r="G5" t="n">
-        <v>0.7106</v>
+        <v>0.30576</v>
       </c>
       <c r="H5" t="n">
-        <v>0.013</v>
+        <v>0.2002</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0192</v>
+        <v>0.12558</v>
       </c>
       <c r="J5" t="n">
-        <v>0.0168</v>
+        <v>0.09645999999999999</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0126</v>
+        <v>0.080535</v>
       </c>
       <c r="L5" t="n">
-        <v>0.004714</v>
+        <v>0.02929745</v>
       </c>
       <c r="M5" t="n">
-        <v>0.005944</v>
+        <v>0.01345435</v>
       </c>
       <c r="N5" t="n">
-        <v>392.4</v>
+        <v>182.91</v>
       </c>
       <c r="O5" t="n">
-        <v>8655</v>
+        <v>4016.74</v>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Recipe 2</t>
+          <t>Rice and chicken</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Soybean Tofu</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.125215</v>
+        <v>0.4186</v>
       </c>
       <c r="C6" t="n">
-        <v>0.309855</v>
+        <v>0.0616</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0.43589</v>
+        <v>-0.004399999999999999</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.225225</v>
+        <v>0.7106</v>
       </c>
       <c r="H6" t="n">
-        <v>0.36127</v>
+        <v>0.013</v>
       </c>
       <c r="I6" t="n">
-        <v>0.080535</v>
+        <v>0.0192</v>
       </c>
       <c r="J6" t="n">
-        <v>0.080535</v>
+        <v>0.0168</v>
       </c>
       <c r="K6" t="n">
-        <v>0.12285</v>
+        <v>0.0126</v>
       </c>
       <c r="L6" t="n">
-        <v>0.00284375</v>
+        <v>0.004714</v>
       </c>
       <c r="M6" t="n">
-        <v>0.00251615</v>
+        <v>0.005944</v>
       </c>
       <c r="N6" t="n">
-        <v>63.245</v>
+        <v>392.4</v>
       </c>
       <c r="O6" t="n">
-        <v>2177.175</v>
+        <v>8655</v>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Recipe 2</t>
+          <t>Rice and Soy tofu</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>Soybean Tofu</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.543815</v>
+        <v>1.125215</v>
       </c>
       <c r="C7" t="n">
-        <v>0.371455</v>
+        <v>0.309855</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.43149</v>
+        <v>0.43589</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.935825</v>
+        <v>0.225225</v>
       </c>
       <c r="H7" t="n">
-        <v>0.37427</v>
+        <v>0.36127</v>
       </c>
       <c r="I7" t="n">
-        <v>0.09973499999999999</v>
+        <v>0.080535</v>
       </c>
       <c r="J7" t="n">
-        <v>0.097335</v>
+        <v>0.080535</v>
       </c>
       <c r="K7" t="n">
-        <v>0.13545</v>
+        <v>0.12285</v>
       </c>
       <c r="L7" t="n">
-        <v>0.00755775</v>
+        <v>0.00284375</v>
       </c>
       <c r="M7" t="n">
-        <v>0.00846015</v>
+        <v>0.00251615</v>
       </c>
       <c r="N7" t="n">
-        <v>455.645</v>
+        <v>63.245</v>
       </c>
       <c r="O7" t="n">
-        <v>10832.175</v>
+        <v>2177.175</v>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Recipe 2</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Rice</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0.4186</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.0616</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>-0.004399999999999999</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.7106</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.013</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.0192</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.0168</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.0126</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0.004714</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.005944</v>
-      </c>
-      <c r="N8" t="n">
-        <v>392.4</v>
-      </c>
-      <c r="O8" t="n">
-        <v>8655</v>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>Recipe 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Chicken</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>2.5753</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.83265</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="n">
-        <v>1.1557</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.807625</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.30576</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.2002</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.12558</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.09645999999999999</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0.080535</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0.02929745</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0.01345435</v>
-      </c>
-      <c r="N9" t="n">
-        <v>182.91</v>
-      </c>
-      <c r="O9" t="n">
-        <v>4016.74</v>
-      </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>Recipe 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>2.9939</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.89425</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="n">
-        <v>1.1513</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.807625</v>
-      </c>
-      <c r="G10" t="n">
-        <v>1.01636</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.2132</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.14478</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0.11326</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0.093135</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0.03401145000000001</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0.01939835</v>
-      </c>
-      <c r="N10" t="n">
-        <v>575.3099999999999</v>
-      </c>
-      <c r="O10" t="n">
-        <v>12671.74</v>
-      </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>Recipe 3</t>
+          <t>Rice and Soy tofu</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating the constacts file
</commit_message>
<xml_diff>
--- a/data/interim/Impacts_per_ingredients.xlsx
+++ b/data/interim/Impacts_per_ingredients.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:P79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,998 +518,1026 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Sunflower oil</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.5866992</v>
+        <v>0.8372000000000001</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1560816</v>
+        <v>0.1232</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.005745600000000001</v>
+        <v>-0.008799999999999999</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.09279360000000002</v>
+        <v>1.4212</v>
       </c>
       <c r="H2" t="n">
-        <v>0.009892800000000002</v>
+        <v>0.026</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0086832</v>
+        <v>0.0384</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0368496</v>
+        <v>0.0336</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0018576</v>
+        <v>0.0252</v>
       </c>
       <c r="L2" t="n">
-        <v>0.00118152</v>
+        <v>0.009428000000000001</v>
       </c>
       <c r="M2" t="n">
-        <v>0.002186352</v>
+        <v>0.011888</v>
       </c>
       <c r="N2" t="n">
-        <v>40.73760000000001</v>
+        <v>784.8</v>
       </c>
       <c r="O2" t="n">
-        <v>1471.5648</v>
+        <v>17310</v>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Chicken in creme freice</t>
+          <t>Lomo Saltado with beef</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Onions</t>
+          <t>French fries</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.07227</v>
+        <v>0.22659</v>
       </c>
       <c r="C3" t="n">
-        <v>0.02178</v>
+        <v>0.06597499999999999</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.00165</v>
+        <v>-0.000455</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0.06963</v>
+        <v>0.087815</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0.03135</v>
+        <v>0.04277</v>
       </c>
       <c r="J3" t="n">
-        <v>0.01485</v>
+        <v>0.020475</v>
       </c>
       <c r="K3" t="n">
-        <v>0.01287</v>
+        <v>0.017745</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0010032</v>
+        <v>0.00146965</v>
       </c>
       <c r="M3" t="n">
-        <v>0.000759</v>
+        <v>0.00116025</v>
       </c>
       <c r="N3" t="n">
-        <v>3.63</v>
+        <v>19.565</v>
       </c>
       <c r="O3" t="n">
-        <v>246.18</v>
+        <v>922.285</v>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Chicken in creme freice</t>
+          <t>Lomo Saltado with beef</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sweet pepper</t>
+          <t>Olive oil</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.0669</v>
+        <v>1.5021576</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0261</v>
+        <v>0.0601128</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0003</v>
+        <v>-0.0208104</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0522</v>
+        <v>0.2358144</v>
       </c>
       <c r="H4" t="n">
-        <v>0.018</v>
+        <v>0.036432</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0492</v>
+        <v>0.0266064</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0123</v>
+        <v>0.0475272</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0045</v>
+        <v>0.0025392</v>
       </c>
       <c r="L4" t="n">
-        <v>0.001593</v>
+        <v>0.002267616</v>
       </c>
       <c r="M4" t="n">
-        <v>0.000558</v>
+        <v>0.002221248</v>
       </c>
       <c r="N4" t="n">
-        <v>24.9</v>
+        <v>128.1744</v>
       </c>
       <c r="O4" t="n">
-        <v>1187.4</v>
+        <v>10638.0888</v>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>Chicken in creme freice</t>
+          <t>Lomo Saltado with beef</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Mushrooms</t>
+          <t>Tomatoes</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1115</v>
+        <v>0.0984</v>
       </c>
       <c r="C5" t="n">
+        <v>0.0546</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.1116</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.2112</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.0036</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.05309999999999999</v>
+      </c>
+      <c r="J5" t="n">
         <v>0.0435</v>
       </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.0005</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.08699999999999999</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.082</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.0205</v>
-      </c>
       <c r="K5" t="n">
-        <v>0.0075</v>
+        <v>0.0051</v>
       </c>
       <c r="L5" t="n">
-        <v>0.002655</v>
+        <v>0.003429</v>
       </c>
       <c r="M5" t="n">
-        <v>0.0009300000000000001</v>
+        <v>0.001443</v>
       </c>
       <c r="N5" t="n">
-        <v>41.5</v>
+        <v>70.5</v>
       </c>
       <c r="O5" t="n">
-        <v>1979</v>
+        <v>1203.9</v>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Chicken in creme freice</t>
+          <t>Lomo Saltado with beef</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Chicken</t>
+          <t>Onions</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4.528</v>
+        <v>0.02409</v>
       </c>
       <c r="C6" t="n">
-        <v>1.464</v>
+        <v>0.007260000000000001</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>2.032</v>
+        <v>0.00055</v>
       </c>
       <c r="F6" t="n">
-        <v>1.42</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.5376000000000001</v>
+        <v>0.02321</v>
       </c>
       <c r="H6" t="n">
-        <v>0.352</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0.2208</v>
+        <v>0.01045</v>
       </c>
       <c r="J6" t="n">
-        <v>0.1696</v>
+        <v>0.00495</v>
       </c>
       <c r="K6" t="n">
-        <v>0.1416</v>
+        <v>0.00429</v>
       </c>
       <c r="L6" t="n">
-        <v>0.051512</v>
+        <v>0.0003344000000000001</v>
       </c>
       <c r="M6" t="n">
-        <v>0.023656</v>
+        <v>0.000253</v>
       </c>
       <c r="N6" t="n">
-        <v>321.6</v>
+        <v>1.21</v>
       </c>
       <c r="O6" t="n">
-        <v>7062.4</v>
+        <v>82.06</v>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Chicken in creme freice</t>
+          <t>Lomo Saltado with beef</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Pasta</t>
+          <t>Chilli pepper</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.081</v>
+        <v>0.006690000000000001</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3995</v>
+        <v>0.00261</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0805</v>
+        <v>3e-05</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0.372</v>
+        <v>0.00522</v>
       </c>
       <c r="H7" t="n">
-        <v>0.08450000000000001</v>
+        <v>0.0018</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0545</v>
+        <v>0.00492</v>
       </c>
       <c r="J7" t="n">
-        <v>0.0405</v>
+        <v>0.00123</v>
       </c>
       <c r="K7" t="n">
-        <v>0.0245</v>
+        <v>0.0004499999999999999</v>
       </c>
       <c r="L7" t="n">
-        <v>0.00526</v>
+        <v>0.0001593</v>
       </c>
       <c r="M7" t="n">
-        <v>0.002845</v>
+        <v>5.58e-05</v>
       </c>
       <c r="N7" t="n">
-        <v>219</v>
+        <v>2.49</v>
       </c>
       <c r="O7" t="n">
-        <v>11131</v>
+        <v>118.74</v>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Chicken in creme freice</t>
+          <t>Lomo Saltado with beef</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Spices Misc.</t>
+          <t>Beef</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.30057</v>
+        <v>9.330685000000001</v>
       </c>
       <c r="C8" t="n">
-        <v>0.06995999999999999</v>
+        <v>2.305485</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>76.48186</v>
       </c>
       <c r="E8" t="n">
-        <v>0.18021</v>
+        <v>7.40649</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>0.8544899999999999</v>
       </c>
       <c r="G8" t="n">
-        <v>0.14814</v>
+        <v>17.92154</v>
       </c>
       <c r="H8" t="n">
-        <v>0.007770000000000001</v>
+        <v>0.577395</v>
       </c>
       <c r="I8" t="n">
-        <v>0.00429</v>
+        <v>0.15743</v>
       </c>
       <c r="J8" t="n">
-        <v>0.02241</v>
+        <v>0.112385</v>
       </c>
       <c r="K8" t="n">
-        <v>0.0008999999999999999</v>
+        <v>0.07462000000000001</v>
       </c>
       <c r="L8" t="n">
-        <v>0.0007257</v>
+        <v>0.08612695000000001</v>
       </c>
       <c r="M8" t="n">
-        <v>0.0009611999999999999</v>
+        <v>0.08074885</v>
       </c>
       <c r="N8" t="n">
-        <v>5.16</v>
+        <v>396.305</v>
       </c>
       <c r="O8" t="n">
-        <v>164.58</v>
+        <v>9629.165000000001</v>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Chicken in creme freice</t>
+          <t>Lomo Saltado with beef</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Tomato paste</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
+          <t>Vinegar</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.30057</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.06995999999999999</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.18021</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.14814</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.007770000000000001</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.00429</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.02241</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.0008999999999999999</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.0007257</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.0009611999999999999</v>
+      </c>
+      <c r="N9" t="n">
+        <v>5.16</v>
+      </c>
+      <c r="O9" t="n">
+        <v>164.58</v>
+      </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>Chicken in creme freice</t>
+          <t>Lomo Saltado with beef</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Salt</t>
+          <t>Soy sauce</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.20038</v>
+        <v>0.60114</v>
       </c>
       <c r="C10" t="n">
-        <v>0.04664</v>
+        <v>0.13992</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>0.12014</v>
+        <v>0.36042</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0.09875999999999999</v>
+        <v>0.29628</v>
       </c>
       <c r="H10" t="n">
-        <v>0.00518</v>
+        <v>0.01554</v>
       </c>
       <c r="I10" t="n">
-        <v>0.00286</v>
+        <v>0.008580000000000001</v>
       </c>
       <c r="J10" t="n">
-        <v>0.01494</v>
+        <v>0.04482</v>
       </c>
       <c r="K10" t="n">
-        <v>0.0005999999999999999</v>
+        <v>0.0018</v>
       </c>
       <c r="L10" t="n">
-        <v>0.0004838</v>
+        <v>0.0014514</v>
       </c>
       <c r="M10" t="n">
-        <v>0.0006408000000000001</v>
+        <v>0.0019224</v>
       </c>
       <c r="N10" t="n">
-        <v>3.44</v>
+        <v>10.32</v>
       </c>
       <c r="O10" t="n">
-        <v>109.72</v>
+        <v>329.16</v>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Chicken in creme freice</t>
+          <t>Lomo Saltado with beef</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Black pepper</t>
+          <t>Coriander</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.20038</v>
+        <v>0.040076</v>
       </c>
       <c r="C11" t="n">
-        <v>0.04664</v>
+        <v>0.009327999999999999</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>0.12014</v>
+        <v>0.024028</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0.09875999999999999</v>
+        <v>0.019752</v>
       </c>
       <c r="H11" t="n">
-        <v>0.00518</v>
+        <v>0.001036</v>
       </c>
       <c r="I11" t="n">
-        <v>0.00286</v>
+        <v>0.0005719999999999999</v>
       </c>
       <c r="J11" t="n">
-        <v>0.01494</v>
+        <v>0.002988</v>
       </c>
       <c r="K11" t="n">
-        <v>0.0005999999999999999</v>
+        <v>0.00012</v>
       </c>
       <c r="L11" t="n">
-        <v>0.0004838</v>
+        <v>9.676e-05</v>
       </c>
       <c r="M11" t="n">
-        <v>0.0006408000000000001</v>
+        <v>0.00012816</v>
       </c>
       <c r="N11" t="n">
-        <v>3.44</v>
+        <v>0.6879999999999999</v>
       </c>
       <c r="O11" t="n">
-        <v>109.72</v>
+        <v>21.944</v>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Chicken in creme freice</t>
+          <t>Lomo Saltado with beef</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Cream</t>
+          <t>Garlic</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.45118</v>
+        <v>0.150285</v>
       </c>
       <c r="C12" t="n">
-        <v>0.13668</v>
+        <v>0.03498</v>
       </c>
       <c r="D12" t="n">
-        <v>2.1335</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1683</v>
+        <v>0.09010499999999999</v>
       </c>
       <c r="F12" t="n">
-        <v>0.08023999999999999</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0.49572</v>
+        <v>0.07407</v>
       </c>
       <c r="H12" t="n">
-        <v>0.05066</v>
+        <v>0.003885</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0306</v>
+        <v>0.002145</v>
       </c>
       <c r="J12" t="n">
-        <v>0.03298</v>
+        <v>0.011205</v>
       </c>
       <c r="K12" t="n">
-        <v>0.08704000000000001</v>
+        <v>0.0004499999999999999</v>
       </c>
       <c r="L12" t="n">
-        <v>0.006004399999999999</v>
+        <v>0.00036285</v>
       </c>
       <c r="M12" t="n">
-        <v>0.0031756</v>
+        <v>0.0004806</v>
       </c>
       <c r="N12" t="n">
-        <v>181.22</v>
+        <v>2.58</v>
       </c>
       <c r="O12" t="n">
-        <v>5763.34</v>
+        <v>82.29000000000001</v>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>Chicken in creme freice</t>
+          <t>Lomo Saltado with beef</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Jasmine rice</t>
+          <t>Salt</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.6279</v>
+        <v>0.20038</v>
       </c>
       <c r="C13" t="n">
-        <v>0.09240000000000001</v>
+        <v>0.04664</v>
       </c>
       <c r="D13" t="n">
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.0066</v>
+        <v>0.12014</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>1.0659</v>
+        <v>0.09875999999999999</v>
       </c>
       <c r="H13" t="n">
-        <v>0.0195</v>
+        <v>0.00518</v>
       </c>
       <c r="I13" t="n">
-        <v>0.0288</v>
+        <v>0.00286</v>
       </c>
       <c r="J13" t="n">
-        <v>0.0252</v>
+        <v>0.01494</v>
       </c>
       <c r="K13" t="n">
-        <v>0.0189</v>
+        <v>0.0005999999999999999</v>
       </c>
       <c r="L13" t="n">
-        <v>0.007071000000000001</v>
+        <v>0.0004838</v>
       </c>
       <c r="M13" t="n">
-        <v>0.008916</v>
+        <v>0.0006408000000000001</v>
       </c>
       <c r="N13" t="n">
-        <v>588.6</v>
+        <v>3.44</v>
       </c>
       <c r="O13" t="n">
-        <v>12982.5</v>
+        <v>109.72</v>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Chilli con carne</t>
+          <t>Lomo Saltado with beef</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Red kidney beans</t>
+          <t>Black pepper</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>3.9404</v>
+        <v>0.40076</v>
       </c>
       <c r="C14" t="n">
-        <v>1.5076</v>
+        <v>0.09328</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>0.0132</v>
+        <v>0.24028</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>0.4356</v>
+        <v>0.19752</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>0.01036</v>
       </c>
       <c r="I14" t="n">
-        <v>0.0384</v>
+        <v>0.005719999999999999</v>
       </c>
       <c r="J14" t="n">
-        <v>0.1412</v>
+        <v>0.02988</v>
       </c>
       <c r="K14" t="n">
-        <v>0.0156</v>
+        <v>0.0012</v>
       </c>
       <c r="L14" t="n">
-        <v>0.007652</v>
+        <v>0.0009676</v>
       </c>
       <c r="M14" t="n">
-        <v>0.006004000000000001</v>
+        <v>0.0012816</v>
       </c>
       <c r="N14" t="n">
-        <v>145.6</v>
+        <v>6.88</v>
       </c>
       <c r="O14" t="n">
-        <v>7468</v>
+        <v>219.44</v>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Chilli con carne</t>
+          <t>Lomo Saltado with beef</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Sunflower oil</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.5866992</v>
+        <v>0.8372000000000001</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1560816</v>
+        <v>0.1232</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>0.005745600000000001</v>
+        <v>-0.008799999999999999</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>0.09279360000000002</v>
+        <v>1.4212</v>
       </c>
       <c r="H15" t="n">
-        <v>0.009892800000000002</v>
+        <v>0.026</v>
       </c>
       <c r="I15" t="n">
-        <v>0.0086832</v>
+        <v>0.0384</v>
       </c>
       <c r="J15" t="n">
-        <v>0.0368496</v>
+        <v>0.0336</v>
       </c>
       <c r="K15" t="n">
-        <v>0.0018576</v>
+        <v>0.0252</v>
       </c>
       <c r="L15" t="n">
-        <v>0.00118152</v>
+        <v>0.009428000000000001</v>
       </c>
       <c r="M15" t="n">
-        <v>0.002186352</v>
+        <v>0.011888</v>
       </c>
       <c r="N15" t="n">
-        <v>40.73760000000001</v>
+        <v>784.8</v>
       </c>
       <c r="O15" t="n">
-        <v>1471.5648</v>
+        <v>17310</v>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Chilli con carne</t>
+          <t>Lomo Saltado with chicken</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Onions</t>
+          <t>French fries</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.07227</v>
+        <v>0.22659</v>
       </c>
       <c r="C16" t="n">
-        <v>0.02178</v>
+        <v>0.06597499999999999</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>0.00165</v>
+        <v>-0.000455</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>0.06963</v>
+        <v>0.087815</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>0.03135</v>
+        <v>0.04277</v>
       </c>
       <c r="J16" t="n">
-        <v>0.01485</v>
+        <v>0.020475</v>
       </c>
       <c r="K16" t="n">
-        <v>0.01287</v>
+        <v>0.017745</v>
       </c>
       <c r="L16" t="n">
-        <v>0.0010032</v>
+        <v>0.00146965</v>
       </c>
       <c r="M16" t="n">
-        <v>0.000759</v>
+        <v>0.00116025</v>
       </c>
       <c r="N16" t="n">
-        <v>3.63</v>
+        <v>19.565</v>
       </c>
       <c r="O16" t="n">
-        <v>246.18</v>
+        <v>922.285</v>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>Chilli con carne</t>
+          <t>Lomo Saltado with chicken</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Chilli pepper</t>
+          <t>Olive oil</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.006690000000000001</v>
+        <v>1.5021576</v>
       </c>
       <c r="C17" t="n">
-        <v>0.00261</v>
+        <v>0.0601128</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>3e-05</v>
+        <v>-0.0208104</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>0.00522</v>
+        <v>0.2358144</v>
       </c>
       <c r="H17" t="n">
-        <v>0.0018</v>
+        <v>0.036432</v>
       </c>
       <c r="I17" t="n">
-        <v>0.00492</v>
+        <v>0.0266064</v>
       </c>
       <c r="J17" t="n">
-        <v>0.00123</v>
+        <v>0.0475272</v>
       </c>
       <c r="K17" t="n">
-        <v>0.0004499999999999999</v>
+        <v>0.0025392</v>
       </c>
       <c r="L17" t="n">
-        <v>0.0001593</v>
+        <v>0.002267616</v>
       </c>
       <c r="M17" t="n">
-        <v>5.58e-05</v>
+        <v>0.002221248</v>
       </c>
       <c r="N17" t="n">
-        <v>2.49</v>
+        <v>128.1744</v>
       </c>
       <c r="O17" t="n">
-        <v>118.74</v>
+        <v>10638.0888</v>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>Chilli con carne</t>
+          <t>Lomo Saltado with chicken</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Sweet corn</t>
+          <t>Tomatoes</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.0446</v>
+        <v>0.0984</v>
       </c>
       <c r="C18" t="n">
-        <v>0.0174</v>
+        <v>0.0546</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>0.0002</v>
+        <v>0.1116</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>0.0348</v>
+        <v>0.2112</v>
       </c>
       <c r="H18" t="n">
-        <v>0.012</v>
+        <v>0.0036</v>
       </c>
       <c r="I18" t="n">
-        <v>0.0328</v>
+        <v>0.05309999999999999</v>
       </c>
       <c r="J18" t="n">
-        <v>0.008200000000000001</v>
+        <v>0.0435</v>
       </c>
       <c r="K18" t="n">
-        <v>0.003</v>
+        <v>0.0051</v>
       </c>
       <c r="L18" t="n">
-        <v>0.001062</v>
+        <v>0.003429</v>
       </c>
       <c r="M18" t="n">
-        <v>0.000372</v>
+        <v>0.001443</v>
       </c>
       <c r="N18" t="n">
-        <v>16.6</v>
+        <v>70.5</v>
       </c>
       <c r="O18" t="n">
-        <v>791.6</v>
+        <v>1203.9</v>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Chilli con carne</t>
+          <t>Lomo Saltado with chicken</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Sweet pepper</t>
+          <t>Onions</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.0669</v>
+        <v>0.02409</v>
       </c>
       <c r="C19" t="n">
-        <v>0.0261</v>
+        <v>0.007260000000000001</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0003</v>
+        <v>0.00055</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>0.0522</v>
+        <v>0.02321</v>
       </c>
       <c r="H19" t="n">
-        <v>0.018</v>
+        <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0492</v>
+        <v>0.01045</v>
       </c>
       <c r="J19" t="n">
-        <v>0.0123</v>
+        <v>0.00495</v>
       </c>
       <c r="K19" t="n">
-        <v>0.0045</v>
+        <v>0.00429</v>
       </c>
       <c r="L19" t="n">
-        <v>0.001593</v>
+        <v>0.0003344000000000001</v>
       </c>
       <c r="M19" t="n">
-        <v>0.000558</v>
+        <v>0.000253</v>
       </c>
       <c r="N19" t="n">
-        <v>24.9</v>
+        <v>1.21</v>
       </c>
       <c r="O19" t="n">
-        <v>1187.4</v>
+        <v>82.06</v>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>Chilli con carne</t>
+          <t>Lomo Saltado with chicken</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Mushrooms</t>
+          <t>Chilli pepper</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.0892</v>
+        <v>0.006690000000000001</v>
       </c>
       <c r="C20" t="n">
-        <v>0.0348</v>
+        <v>0.00261</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>0.0004</v>
+        <v>3e-05</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
       </c>
       <c r="G20" t="n">
-        <v>0.0696</v>
+        <v>0.00522</v>
       </c>
       <c r="H20" t="n">
-        <v>0.024</v>
+        <v>0.0018</v>
       </c>
       <c r="I20" t="n">
-        <v>0.06560000000000001</v>
+        <v>0.00492</v>
       </c>
       <c r="J20" t="n">
-        <v>0.0164</v>
+        <v>0.00123</v>
       </c>
       <c r="K20" t="n">
-        <v>0.006</v>
+        <v>0.0004499999999999999</v>
       </c>
       <c r="L20" t="n">
-        <v>0.002124</v>
+        <v>0.0001593</v>
       </c>
       <c r="M20" t="n">
-        <v>0.000744</v>
+        <v>5.58e-05</v>
       </c>
       <c r="N20" t="n">
-        <v>33.2</v>
+        <v>2.49</v>
       </c>
       <c r="O20" t="n">
-        <v>1583.2</v>
+        <v>118.74</v>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Chilli con carne</t>
+          <t>Lomo Saltado with chicken</t>
         </is>
       </c>
     </row>
@@ -1520,1400 +1548,3182 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>4.528</v>
+        <v>2.5753</v>
       </c>
       <c r="C21" t="n">
-        <v>1.464</v>
+        <v>0.83265</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>2.032</v>
+        <v>1.1557</v>
       </c>
       <c r="F21" t="n">
-        <v>1.42</v>
+        <v>0.807625</v>
       </c>
       <c r="G21" t="n">
-        <v>0.5376000000000001</v>
+        <v>0.30576</v>
       </c>
       <c r="H21" t="n">
-        <v>0.352</v>
+        <v>0.2002</v>
       </c>
       <c r="I21" t="n">
-        <v>0.2208</v>
+        <v>0.12558</v>
       </c>
       <c r="J21" t="n">
-        <v>0.1696</v>
+        <v>0.09645999999999999</v>
       </c>
       <c r="K21" t="n">
-        <v>0.1416</v>
+        <v>0.080535</v>
       </c>
       <c r="L21" t="n">
-        <v>0.051512</v>
+        <v>0.02929745</v>
       </c>
       <c r="M21" t="n">
-        <v>0.023656</v>
+        <v>0.01345435</v>
       </c>
       <c r="N21" t="n">
-        <v>321.6</v>
+        <v>182.91</v>
       </c>
       <c r="O21" t="n">
-        <v>7062.4</v>
+        <v>4016.74</v>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Chilli con carne</t>
+          <t>Lomo Saltado with chicken</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Tomato sauce</t>
+          <t>Vinegar</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>8.0152</v>
+        <v>0.30057</v>
       </c>
       <c r="C22" t="n">
-        <v>1.8656</v>
+        <v>0.06995999999999999</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>4.805599999999999</v>
+        <v>0.18021</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>3.9504</v>
+        <v>0.14814</v>
       </c>
       <c r="H22" t="n">
-        <v>0.2072</v>
+        <v>0.007770000000000001</v>
       </c>
       <c r="I22" t="n">
-        <v>0.1144</v>
+        <v>0.00429</v>
       </c>
       <c r="J22" t="n">
-        <v>0.5976</v>
+        <v>0.02241</v>
       </c>
       <c r="K22" t="n">
-        <v>0.024</v>
+        <v>0.0008999999999999999</v>
       </c>
       <c r="L22" t="n">
-        <v>0.019352</v>
+        <v>0.0007257</v>
       </c>
       <c r="M22" t="n">
-        <v>0.025632</v>
+        <v>0.0009611999999999999</v>
       </c>
       <c r="N22" t="n">
-        <v>137.6</v>
+        <v>5.16</v>
       </c>
       <c r="O22" t="n">
-        <v>4388.8</v>
+        <v>164.58</v>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Chilli con carne</t>
+          <t>Lomo Saltado with chicken</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Salt</t>
+          <t>Soy sauce</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.20038</v>
+        <v>0.60114</v>
       </c>
       <c r="C23" t="n">
-        <v>0.04664</v>
+        <v>0.13992</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>0.12014</v>
+        <v>0.36042</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
       </c>
       <c r="G23" t="n">
-        <v>0.09875999999999999</v>
+        <v>0.29628</v>
       </c>
       <c r="H23" t="n">
-        <v>0.00518</v>
+        <v>0.01554</v>
       </c>
       <c r="I23" t="n">
-        <v>0.00286</v>
+        <v>0.008580000000000001</v>
       </c>
       <c r="J23" t="n">
-        <v>0.01494</v>
+        <v>0.04482</v>
       </c>
       <c r="K23" t="n">
-        <v>0.0005999999999999999</v>
+        <v>0.0018</v>
       </c>
       <c r="L23" t="n">
-        <v>0.0004838</v>
+        <v>0.0014514</v>
       </c>
       <c r="M23" t="n">
-        <v>0.0006408000000000001</v>
+        <v>0.0019224</v>
       </c>
       <c r="N23" t="n">
-        <v>3.44</v>
+        <v>10.32</v>
       </c>
       <c r="O23" t="n">
-        <v>109.72</v>
+        <v>329.16</v>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Chilli con carne</t>
+          <t>Lomo Saltado with chicken</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Black pepper</t>
+          <t>Coriander</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.20038</v>
+        <v>0.040076</v>
       </c>
       <c r="C24" t="n">
-        <v>0.04664</v>
+        <v>0.009327999999999999</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>0.12014</v>
+        <v>0.024028</v>
       </c>
       <c r="F24" t="n">
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>0.09875999999999999</v>
+        <v>0.019752</v>
       </c>
       <c r="H24" t="n">
-        <v>0.00518</v>
+        <v>0.001036</v>
       </c>
       <c r="I24" t="n">
-        <v>0.00286</v>
+        <v>0.0005719999999999999</v>
       </c>
       <c r="J24" t="n">
-        <v>0.01494</v>
+        <v>0.002988</v>
       </c>
       <c r="K24" t="n">
-        <v>0.0005999999999999999</v>
+        <v>0.00012</v>
       </c>
       <c r="L24" t="n">
-        <v>0.0004838</v>
+        <v>9.676e-05</v>
       </c>
       <c r="M24" t="n">
-        <v>0.0006408000000000001</v>
+        <v>0.00012816</v>
       </c>
       <c r="N24" t="n">
-        <v>3.44</v>
+        <v>0.6879999999999999</v>
       </c>
       <c r="O24" t="n">
-        <v>109.72</v>
+        <v>21.944</v>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Chilli con carne</t>
+          <t>Lomo Saltado with chicken</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Sweet potatoes</t>
+          <t>Garlic</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.5976</v>
+        <v>0.150285</v>
       </c>
       <c r="C25" t="n">
-        <v>0.174</v>
+        <v>0.03498</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>-0.0012</v>
+        <v>0.09010499999999999</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>0.2316</v>
+        <v>0.07407</v>
       </c>
       <c r="H25" t="n">
-        <v>0</v>
+        <v>0.003885</v>
       </c>
       <c r="I25" t="n">
-        <v>0.1128</v>
+        <v>0.002145</v>
       </c>
       <c r="J25" t="n">
-        <v>0.054</v>
+        <v>0.011205</v>
       </c>
       <c r="K25" t="n">
-        <v>0.04679999999999999</v>
+        <v>0.0004499999999999999</v>
       </c>
       <c r="L25" t="n">
-        <v>0.003876</v>
+        <v>0.00036285</v>
       </c>
       <c r="M25" t="n">
-        <v>0.00306</v>
+        <v>0.0004806</v>
       </c>
       <c r="N25" t="n">
-        <v>51.6</v>
+        <v>2.58</v>
       </c>
       <c r="O25" t="n">
-        <v>2432.4</v>
+        <v>82.29000000000001</v>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Kylling og søtpotet</t>
+          <t>Lomo Saltado with chicken</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Onions</t>
+          <t>Salt</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.09636</v>
+        <v>0.20038</v>
       </c>
       <c r="C26" t="n">
-        <v>0.02904</v>
+        <v>0.04664</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>0.0022</v>
+        <v>0.12014</v>
       </c>
       <c r="F26" t="n">
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>0.09284000000000001</v>
+        <v>0.09875999999999999</v>
       </c>
       <c r="H26" t="n">
-        <v>0</v>
+        <v>0.00518</v>
       </c>
       <c r="I26" t="n">
-        <v>0.0418</v>
+        <v>0.00286</v>
       </c>
       <c r="J26" t="n">
-        <v>0.0198</v>
+        <v>0.01494</v>
       </c>
       <c r="K26" t="n">
-        <v>0.01716</v>
+        <v>0.0005999999999999999</v>
       </c>
       <c r="L26" t="n">
-        <v>0.0013376</v>
+        <v>0.0004838</v>
       </c>
       <c r="M26" t="n">
-        <v>0.001012</v>
+        <v>0.0006408000000000001</v>
       </c>
       <c r="N26" t="n">
-        <v>4.84</v>
+        <v>3.44</v>
       </c>
       <c r="O26" t="n">
-        <v>328.24</v>
+        <v>109.72</v>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Kylling og søtpotet</t>
+          <t>Lomo Saltado with chicken</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Broccoli</t>
+          <t>Black pepper</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.2424</v>
+        <v>0.40076</v>
       </c>
       <c r="C27" t="n">
-        <v>0.1192</v>
+        <v>0.09328</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>0.0016</v>
+        <v>0.24028</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>0.2224</v>
+        <v>0.19752</v>
       </c>
       <c r="H27" t="n">
-        <v>0</v>
+        <v>0.01036</v>
       </c>
       <c r="I27" t="n">
-        <v>0.076</v>
+        <v>0.005719999999999999</v>
       </c>
       <c r="J27" t="n">
-        <v>0.036</v>
+        <v>0.02988</v>
       </c>
       <c r="K27" t="n">
-        <v>0.0136</v>
+        <v>0.0012</v>
       </c>
       <c r="L27" t="n">
-        <v>0.005488</v>
+        <v>0.0009676</v>
       </c>
       <c r="M27" t="n">
-        <v>0.003312</v>
+        <v>0.0012816</v>
       </c>
       <c r="N27" t="n">
-        <v>77.59999999999999</v>
+        <v>6.88</v>
       </c>
       <c r="O27" t="n">
-        <v>5502.4</v>
+        <v>219.44</v>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Kylling og søtpotet</t>
+          <t>Lomo Saltado with chicken</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Chicken</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>4.528</v>
+        <v>0.8372000000000001</v>
       </c>
       <c r="C28" t="n">
-        <v>1.464</v>
+        <v>0.1232</v>
       </c>
       <c r="D28" t="n">
         <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>2.032</v>
+        <v>-0.008799999999999999</v>
       </c>
       <c r="F28" t="n">
-        <v>1.42</v>
+        <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>0.5376000000000001</v>
+        <v>1.4212</v>
       </c>
       <c r="H28" t="n">
-        <v>0.352</v>
+        <v>0.026</v>
       </c>
       <c r="I28" t="n">
-        <v>0.2208</v>
+        <v>0.0384</v>
       </c>
       <c r="J28" t="n">
-        <v>0.1696</v>
+        <v>0.0336</v>
       </c>
       <c r="K28" t="n">
-        <v>0.1416</v>
+        <v>0.0252</v>
       </c>
       <c r="L28" t="n">
-        <v>0.051512</v>
+        <v>0.009428000000000001</v>
       </c>
       <c r="M28" t="n">
-        <v>0.023656</v>
+        <v>0.011888</v>
       </c>
       <c r="N28" t="n">
-        <v>321.6</v>
+        <v>784.8</v>
       </c>
       <c r="O28" t="n">
-        <v>7062.4</v>
+        <v>17310</v>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Kylling og søtpotet</t>
+          <t>Lomo Saltado with chickpeas</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Salt</t>
+          <t>French fries</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.20038</v>
+        <v>0.22659</v>
       </c>
       <c r="C29" t="n">
-        <v>0.04664</v>
+        <v>0.06597499999999999</v>
       </c>
       <c r="D29" t="n">
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>0.12014</v>
+        <v>-0.000455</v>
       </c>
       <c r="F29" t="n">
         <v>0</v>
       </c>
       <c r="G29" t="n">
-        <v>0.09875999999999999</v>
+        <v>0.087815</v>
       </c>
       <c r="H29" t="n">
-        <v>0.00518</v>
+        <v>0</v>
       </c>
       <c r="I29" t="n">
-        <v>0.00286</v>
+        <v>0.04277</v>
       </c>
       <c r="J29" t="n">
-        <v>0.01494</v>
+        <v>0.020475</v>
       </c>
       <c r="K29" t="n">
-        <v>0.0005999999999999999</v>
+        <v>0.017745</v>
       </c>
       <c r="L29" t="n">
-        <v>0.0004838</v>
+        <v>0.00146965</v>
       </c>
       <c r="M29" t="n">
-        <v>0.0006408000000000001</v>
+        <v>0.00116025</v>
       </c>
       <c r="N29" t="n">
-        <v>3.44</v>
+        <v>19.565</v>
       </c>
       <c r="O29" t="n">
-        <v>109.72</v>
+        <v>922.285</v>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Kylling og søtpotet</t>
+          <t>Lomo Saltado with chickpeas</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Black pepper</t>
+          <t>Chickpeas</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.20038</v>
+        <v>4.482205</v>
       </c>
       <c r="C30" t="n">
-        <v>0.04664</v>
+        <v>1.714895</v>
       </c>
       <c r="D30" t="n">
         <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>0.12014</v>
+        <v>0.015015</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>0.09875999999999999</v>
+        <v>0.495495</v>
       </c>
       <c r="H30" t="n">
-        <v>0.00518</v>
+        <v>0</v>
       </c>
       <c r="I30" t="n">
-        <v>0.00286</v>
+        <v>0.04368</v>
       </c>
       <c r="J30" t="n">
-        <v>0.01494</v>
+        <v>0.160615</v>
       </c>
       <c r="K30" t="n">
-        <v>0.0005999999999999999</v>
+        <v>0.017745</v>
       </c>
       <c r="L30" t="n">
-        <v>0.0004838</v>
+        <v>0.008704150000000001</v>
       </c>
       <c r="M30" t="n">
-        <v>0.0006408000000000001</v>
+        <v>0.00682955</v>
       </c>
       <c r="N30" t="n">
-        <v>3.44</v>
+        <v>165.62</v>
       </c>
       <c r="O30" t="n">
-        <v>109.72</v>
+        <v>8494.85</v>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Kylling og søtpotet</t>
+          <t>Lomo Saltado with chickpeas</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Potatoes</t>
+          <t>Olive oil</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.7968</v>
+        <v>1.5021576</v>
       </c>
       <c r="C31" t="n">
-        <v>0.232</v>
+        <v>0.0601128</v>
       </c>
       <c r="D31" t="n">
         <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>-0.0016</v>
+        <v>-0.0208104</v>
       </c>
       <c r="F31" t="n">
         <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>0.3088</v>
+        <v>0.2358144</v>
       </c>
       <c r="H31" t="n">
-        <v>0</v>
+        <v>0.036432</v>
       </c>
       <c r="I31" t="n">
-        <v>0.1504</v>
+        <v>0.0266064</v>
       </c>
       <c r="J31" t="n">
-        <v>0.07199999999999999</v>
+        <v>0.0475272</v>
       </c>
       <c r="K31" t="n">
-        <v>0.0624</v>
+        <v>0.0025392</v>
       </c>
       <c r="L31" t="n">
-        <v>0.005167999999999999</v>
+        <v>0.002267616</v>
       </c>
       <c r="M31" t="n">
-        <v>0.00408</v>
+        <v>0.002221248</v>
       </c>
       <c r="N31" t="n">
-        <v>68.8</v>
+        <v>128.1744</v>
       </c>
       <c r="O31" t="n">
-        <v>3243.2</v>
+        <v>10638.0888</v>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Meeeeeat</t>
+          <t>Lomo Saltado with chickpeas</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Onions</t>
+          <t>Tomatoes</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.04818</v>
+        <v>0.0984</v>
       </c>
       <c r="C32" t="n">
-        <v>0.01452</v>
+        <v>0.0546</v>
       </c>
       <c r="D32" t="n">
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>0.0011</v>
+        <v>0.1116</v>
       </c>
       <c r="F32" t="n">
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>0.04642</v>
+        <v>0.2112</v>
       </c>
       <c r="H32" t="n">
-        <v>0</v>
+        <v>0.0036</v>
       </c>
       <c r="I32" t="n">
-        <v>0.0209</v>
+        <v>0.05309999999999999</v>
       </c>
       <c r="J32" t="n">
-        <v>0.009900000000000001</v>
+        <v>0.0435</v>
       </c>
       <c r="K32" t="n">
-        <v>0.008580000000000001</v>
+        <v>0.0051</v>
       </c>
       <c r="L32" t="n">
-        <v>0.0006688000000000001</v>
+        <v>0.003429</v>
       </c>
       <c r="M32" t="n">
-        <v>0.000506</v>
+        <v>0.001443</v>
       </c>
       <c r="N32" t="n">
-        <v>2.42</v>
+        <v>70.5</v>
       </c>
       <c r="O32" t="n">
-        <v>164.12</v>
+        <v>1203.9</v>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Meeeeeat</t>
+          <t>Lomo Saltado with chickpeas</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Broccoli</t>
+          <t>Onions</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.2424</v>
+        <v>0.02409</v>
       </c>
       <c r="C33" t="n">
-        <v>0.1192</v>
+        <v>0.007260000000000001</v>
       </c>
       <c r="D33" t="n">
         <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>0.0016</v>
+        <v>0.00055</v>
       </c>
       <c r="F33" t="n">
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>0.2224</v>
+        <v>0.02321</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
       </c>
       <c r="I33" t="n">
-        <v>0.076</v>
+        <v>0.01045</v>
       </c>
       <c r="J33" t="n">
-        <v>0.036</v>
+        <v>0.00495</v>
       </c>
       <c r="K33" t="n">
-        <v>0.0136</v>
+        <v>0.00429</v>
       </c>
       <c r="L33" t="n">
-        <v>0.005488</v>
+        <v>0.0003344000000000001</v>
       </c>
       <c r="M33" t="n">
-        <v>0.003312</v>
+        <v>0.000253</v>
       </c>
       <c r="N33" t="n">
-        <v>77.59999999999999</v>
+        <v>1.21</v>
       </c>
       <c r="O33" t="n">
-        <v>5502.4</v>
+        <v>82.06</v>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Meeeeeat</t>
+          <t>Lomo Saltado with chickpeas</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Cranberries</t>
+          <t>Chilli pepper</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.2964</v>
+        <v>0.006690000000000001</v>
       </c>
       <c r="C34" t="n">
-        <v>0.3596</v>
+        <v>0.00261</v>
       </c>
       <c r="D34" t="n">
         <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>0.01</v>
+        <v>3e-05</v>
       </c>
       <c r="F34" t="n">
         <v>0</v>
       </c>
       <c r="G34" t="n">
-        <v>0.2888</v>
+        <v>0.00522</v>
       </c>
       <c r="H34" t="n">
-        <v>0</v>
+        <v>0.0018</v>
       </c>
       <c r="I34" t="n">
-        <v>0.09519999999999999</v>
+        <v>0.00492</v>
       </c>
       <c r="J34" t="n">
-        <v>0.0848</v>
+        <v>0.00123</v>
       </c>
       <c r="K34" t="n">
-        <v>0.0068</v>
+        <v>0.0004499999999999999</v>
       </c>
       <c r="L34" t="n">
-        <v>0.003956</v>
+        <v>0.0001593</v>
       </c>
       <c r="M34" t="n">
-        <v>0.002124</v>
+        <v>5.58e-05</v>
       </c>
       <c r="N34" t="n">
-        <v>116.8</v>
+        <v>2.49</v>
       </c>
       <c r="O34" t="n">
-        <v>6072</v>
+        <v>118.74</v>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Meeeeeat</t>
+          <t>Lomo Saltado with chickpeas</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Beef</t>
+          <t>Vinegar</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>36.9126</v>
+        <v>0.30057</v>
       </c>
       <c r="C35" t="n">
-        <v>9.1206</v>
+        <v>0.06995999999999999</v>
       </c>
       <c r="D35" t="n">
-        <v>302.5656</v>
+        <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>29.3004</v>
+        <v>0.18021</v>
       </c>
       <c r="F35" t="n">
-        <v>3.3804</v>
+        <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>70.8984</v>
+        <v>0.14814</v>
       </c>
       <c r="H35" t="n">
-        <v>2.2842</v>
+        <v>0.007770000000000001</v>
       </c>
       <c r="I35" t="n">
-        <v>0.6227999999999999</v>
+        <v>0.00429</v>
       </c>
       <c r="J35" t="n">
-        <v>0.4446</v>
+        <v>0.02241</v>
       </c>
       <c r="K35" t="n">
-        <v>0.2952</v>
+        <v>0.0008999999999999999</v>
       </c>
       <c r="L35" t="n">
-        <v>0.340722</v>
+        <v>0.0007257</v>
       </c>
       <c r="M35" t="n">
-        <v>0.319446</v>
+        <v>0.0009611999999999999</v>
       </c>
       <c r="N35" t="n">
-        <v>1567.8</v>
+        <v>5.16</v>
       </c>
       <c r="O35" t="n">
-        <v>38093.4</v>
+        <v>164.58</v>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Meeeeeat</t>
+          <t>Lomo Saltado with chickpeas</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Salt</t>
+          <t>Soy sauce</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.40076</v>
+        <v>0.60114</v>
       </c>
       <c r="C36" t="n">
-        <v>0.09328</v>
+        <v>0.13992</v>
       </c>
       <c r="D36" t="n">
         <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>0.24028</v>
+        <v>0.36042</v>
       </c>
       <c r="F36" t="n">
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>0.19752</v>
+        <v>0.29628</v>
       </c>
       <c r="H36" t="n">
-        <v>0.01036</v>
+        <v>0.01554</v>
       </c>
       <c r="I36" t="n">
-        <v>0.005719999999999999</v>
+        <v>0.008580000000000001</v>
       </c>
       <c r="J36" t="n">
-        <v>0.02988</v>
+        <v>0.04482</v>
       </c>
       <c r="K36" t="n">
-        <v>0.0012</v>
+        <v>0.0018</v>
       </c>
       <c r="L36" t="n">
-        <v>0.0009676</v>
+        <v>0.0014514</v>
       </c>
       <c r="M36" t="n">
-        <v>0.0012816</v>
+        <v>0.0019224</v>
       </c>
       <c r="N36" t="n">
-        <v>6.88</v>
+        <v>10.32</v>
       </c>
       <c r="O36" t="n">
-        <v>219.44</v>
+        <v>329.16</v>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Meeeeeat</t>
+          <t>Lomo Saltado with chickpeas</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Black pepper</t>
+          <t>Coriander</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.40076</v>
+        <v>0.040076</v>
       </c>
       <c r="C37" t="n">
-        <v>0.09328</v>
+        <v>0.009327999999999999</v>
       </c>
       <c r="D37" t="n">
         <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>0.24028</v>
+        <v>0.024028</v>
       </c>
       <c r="F37" t="n">
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>0.19752</v>
+        <v>0.019752</v>
       </c>
       <c r="H37" t="n">
-        <v>0.01036</v>
+        <v>0.001036</v>
       </c>
       <c r="I37" t="n">
-        <v>0.005719999999999999</v>
+        <v>0.0005719999999999999</v>
       </c>
       <c r="J37" t="n">
-        <v>0.02988</v>
+        <v>0.002988</v>
       </c>
       <c r="K37" t="n">
-        <v>0.0012</v>
+        <v>0.00012</v>
       </c>
       <c r="L37" t="n">
-        <v>0.0009676</v>
+        <v>9.676e-05</v>
       </c>
       <c r="M37" t="n">
-        <v>0.0012816</v>
+        <v>0.00012816</v>
       </c>
       <c r="N37" t="n">
-        <v>6.88</v>
+        <v>0.6879999999999999</v>
       </c>
       <c r="O37" t="n">
-        <v>219.44</v>
+        <v>21.944</v>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Meeeeeat</t>
+          <t>Lomo Saltado with chickpeas</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Butter</t>
+          <t>Garlic</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.03981000000000001</v>
+        <v>0.150285</v>
       </c>
       <c r="C38" t="n">
-        <v>0.01206</v>
+        <v>0.03498</v>
       </c>
       <c r="D38" t="n">
-        <v>0.18825</v>
+        <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>0.01485</v>
+        <v>0.09010499999999999</v>
       </c>
       <c r="F38" t="n">
-        <v>0.00708</v>
+        <v>0</v>
       </c>
       <c r="G38" t="n">
-        <v>0.04374</v>
+        <v>0.07407</v>
       </c>
       <c r="H38" t="n">
-        <v>0.00447</v>
+        <v>0.003885</v>
       </c>
       <c r="I38" t="n">
-        <v>0.0027</v>
+        <v>0.002145</v>
       </c>
       <c r="J38" t="n">
-        <v>0.00291</v>
+        <v>0.011205</v>
       </c>
       <c r="K38" t="n">
-        <v>0.007679999999999999</v>
+        <v>0.0004499999999999999</v>
       </c>
       <c r="L38" t="n">
-        <v>0.0005298</v>
+        <v>0.00036285</v>
       </c>
       <c r="M38" t="n">
-        <v>0.0002802</v>
+        <v>0.0004806</v>
       </c>
       <c r="N38" t="n">
-        <v>15.99</v>
+        <v>2.58</v>
       </c>
       <c r="O38" t="n">
-        <v>508.53</v>
+        <v>82.29000000000001</v>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Meeeeeat</t>
+          <t>Lomo Saltado with chickpeas</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Cream</t>
+          <t>Salt</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.45118</v>
+        <v>0.20038</v>
       </c>
       <c r="C39" t="n">
-        <v>0.13668</v>
+        <v>0.04664</v>
       </c>
       <c r="D39" t="n">
-        <v>2.1335</v>
+        <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>0.1683</v>
+        <v>0.12014</v>
       </c>
       <c r="F39" t="n">
-        <v>0.08023999999999999</v>
+        <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>0.49572</v>
+        <v>0.09875999999999999</v>
       </c>
       <c r="H39" t="n">
-        <v>0.05066</v>
+        <v>0.00518</v>
       </c>
       <c r="I39" t="n">
-        <v>0.0306</v>
+        <v>0.00286</v>
       </c>
       <c r="J39" t="n">
-        <v>0.03298</v>
+        <v>0.01494</v>
       </c>
       <c r="K39" t="n">
-        <v>0.08704000000000001</v>
+        <v>0.0005999999999999999</v>
       </c>
       <c r="L39" t="n">
-        <v>0.006004399999999999</v>
+        <v>0.0004838</v>
       </c>
       <c r="M39" t="n">
-        <v>0.0031756</v>
+        <v>0.0006408000000000001</v>
       </c>
       <c r="N39" t="n">
-        <v>181.22</v>
+        <v>3.44</v>
       </c>
       <c r="O39" t="n">
-        <v>5763.34</v>
+        <v>109.72</v>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Meeeeeat</t>
+          <t>Lomo Saltado with chickpeas</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Oats</t>
+          <t>Black pepper</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>5.06979</v>
+        <v>0.40076</v>
       </c>
       <c r="C40" t="n">
-        <v>2.00772</v>
+        <v>0.09328</v>
       </c>
       <c r="D40" t="n">
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>0.001485</v>
+        <v>0.24028</v>
       </c>
       <c r="F40" t="n">
         <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>2.03445</v>
+        <v>0.19752</v>
       </c>
       <c r="H40" t="n">
-        <v>0.06237</v>
+        <v>0.01036</v>
       </c>
       <c r="I40" t="n">
-        <v>0.099495</v>
+        <v>0.005719999999999999</v>
       </c>
       <c r="J40" t="n">
-        <v>0.09801</v>
+        <v>0.02988</v>
       </c>
       <c r="K40" t="n">
-        <v>0.04306500000000001</v>
+        <v>0.0012</v>
       </c>
       <c r="L40" t="n">
-        <v>0.01035045</v>
+        <v>0.0009676</v>
       </c>
       <c r="M40" t="n">
-        <v>0.01046925</v>
+        <v>0.0012816</v>
       </c>
       <c r="N40" t="n">
-        <v>448.47</v>
+        <v>6.88</v>
       </c>
       <c r="O40" t="n">
-        <v>17484.39</v>
+        <v>219.44</v>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Porrige</t>
+          <t>Lomo Saltado with chickpeas</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Soymilk</t>
+          <t>Rice</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.6496000000000001</v>
+        <v>0.8372000000000001</v>
       </c>
       <c r="C41" t="n">
-        <v>0.1792</v>
+        <v>0.1232</v>
       </c>
       <c r="D41" t="n">
         <v>0</v>
       </c>
       <c r="E41" t="n">
-        <v>0.252</v>
+        <v>-0.008799999999999999</v>
       </c>
       <c r="F41" t="n">
         <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>0.1302</v>
+        <v>1.4212</v>
       </c>
       <c r="H41" t="n">
-        <v>0.2282</v>
+        <v>0.026</v>
       </c>
       <c r="I41" t="n">
-        <v>0.154</v>
+        <v>0.0384</v>
       </c>
       <c r="J41" t="n">
-        <v>0.1372</v>
+        <v>0.0336</v>
       </c>
       <c r="K41" t="n">
-        <v>0.378</v>
+        <v>0.0252</v>
       </c>
       <c r="L41" t="n">
-        <v>0.0035</v>
+        <v>0.009428000000000001</v>
       </c>
       <c r="M41" t="n">
-        <v>0.001358</v>
+        <v>0.011888</v>
       </c>
       <c r="N41" t="n">
-        <v>36.4</v>
+        <v>784.8</v>
       </c>
       <c r="O41" t="n">
-        <v>1251.6</v>
+        <v>17310</v>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Porrige</t>
+          <t>Lomo Saltado with mushrooms</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Sunflower seeds</t>
+          <t>French fries</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.6790499999999999</v>
+        <v>0.22659</v>
       </c>
       <c r="C42" t="n">
-        <v>0.18065</v>
+        <v>0.06597499999999999</v>
       </c>
       <c r="D42" t="n">
         <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>0.006650000000000001</v>
+        <v>-0.000455</v>
       </c>
       <c r="F42" t="n">
         <v>0</v>
       </c>
       <c r="G42" t="n">
-        <v>0.1074</v>
+        <v>0.087815</v>
       </c>
       <c r="H42" t="n">
-        <v>0.01145</v>
+        <v>0</v>
       </c>
       <c r="I42" t="n">
-        <v>0.01005</v>
+        <v>0.04277</v>
       </c>
       <c r="J42" t="n">
-        <v>0.04265</v>
+        <v>0.020475</v>
       </c>
       <c r="K42" t="n">
-        <v>0.00215</v>
+        <v>0.017745</v>
       </c>
       <c r="L42" t="n">
-        <v>0.0013675</v>
+        <v>0.00146965</v>
       </c>
       <c r="M42" t="n">
-        <v>0.0025305</v>
+        <v>0.00116025</v>
       </c>
       <c r="N42" t="n">
-        <v>47.15</v>
+        <v>19.565</v>
       </c>
       <c r="O42" t="n">
-        <v>1703.2</v>
+        <v>922.285</v>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Porrige</t>
+          <t>Lomo Saltado with mushrooms</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Bananas</t>
+          <t>Olive oil</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.8856000000000001</v>
+        <v>1.5021576</v>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>0.0601128</v>
       </c>
       <c r="D43" t="n">
         <v>0</v>
       </c>
       <c r="E43" t="n">
-        <v>-0.018</v>
+        <v>-0.0208104</v>
       </c>
       <c r="F43" t="n">
         <v>0</v>
       </c>
       <c r="G43" t="n">
-        <v>0.19152</v>
+        <v>0.2358144</v>
       </c>
       <c r="H43" t="n">
-        <v>0.04248</v>
+        <v>0.036432</v>
       </c>
       <c r="I43" t="n">
-        <v>0.21024</v>
+        <v>0.0266064</v>
       </c>
       <c r="J43" t="n">
-        <v>0.0468</v>
+        <v>0.0475272</v>
       </c>
       <c r="K43" t="n">
-        <v>0.01512</v>
+        <v>0.0025392</v>
       </c>
       <c r="L43" t="n">
-        <v>0.0033768</v>
+        <v>0.002267616</v>
       </c>
       <c r="M43" t="n">
-        <v>0.00162</v>
+        <v>0.002221248</v>
       </c>
       <c r="N43" t="n">
-        <v>61.92</v>
+        <v>128.1744</v>
       </c>
       <c r="O43" t="n">
-        <v>353.52</v>
+        <v>10638.0888</v>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Porrige</t>
+          <t>Lomo Saltado with mushrooms</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Raisin</t>
+          <t>Tomatoes</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.11115</v>
+        <v>0.0984</v>
       </c>
       <c r="C44" t="n">
-        <v>0.13485</v>
+        <v>0.0546</v>
       </c>
       <c r="D44" t="n">
         <v>0</v>
       </c>
       <c r="E44" t="n">
-        <v>0.00375</v>
+        <v>0.1116</v>
       </c>
       <c r="F44" t="n">
         <v>0</v>
       </c>
       <c r="G44" t="n">
-        <v>0.1083</v>
+        <v>0.2112</v>
       </c>
       <c r="H44" t="n">
-        <v>0</v>
+        <v>0.0036</v>
       </c>
       <c r="I44" t="n">
-        <v>0.0357</v>
+        <v>0.05309999999999999</v>
       </c>
       <c r="J44" t="n">
-        <v>0.0318</v>
+        <v>0.0435</v>
       </c>
       <c r="K44" t="n">
-        <v>0.00255</v>
+        <v>0.0051</v>
       </c>
       <c r="L44" t="n">
-        <v>0.0014835</v>
+        <v>0.003429</v>
       </c>
       <c r="M44" t="n">
-        <v>0.0007965</v>
+        <v>0.001443</v>
       </c>
       <c r="N44" t="n">
-        <v>43.8</v>
+        <v>70.5</v>
       </c>
       <c r="O44" t="n">
-        <v>2277</v>
+        <v>1203.9</v>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Porrige</t>
+          <t>Lomo Saltado with mushrooms</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Salt</t>
+          <t>Onions</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.40076</v>
+        <v>0.02409</v>
       </c>
       <c r="C45" t="n">
-        <v>0.09328</v>
+        <v>0.007260000000000001</v>
       </c>
       <c r="D45" t="n">
         <v>0</v>
       </c>
       <c r="E45" t="n">
-        <v>0.24028</v>
+        <v>0.00055</v>
       </c>
       <c r="F45" t="n">
         <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>0.19752</v>
+        <v>0.02321</v>
       </c>
       <c r="H45" t="n">
-        <v>0.01036</v>
+        <v>0</v>
       </c>
       <c r="I45" t="n">
-        <v>0.005719999999999999</v>
+        <v>0.01045</v>
       </c>
       <c r="J45" t="n">
-        <v>0.02988</v>
+        <v>0.00495</v>
       </c>
       <c r="K45" t="n">
-        <v>0.0012</v>
+        <v>0.00429</v>
       </c>
       <c r="L45" t="n">
-        <v>0.0009676</v>
+        <v>0.0003344000000000001</v>
       </c>
       <c r="M45" t="n">
-        <v>0.0012816</v>
+        <v>0.000253</v>
       </c>
       <c r="N45" t="n">
-        <v>6.88</v>
+        <v>1.21</v>
       </c>
       <c r="O45" t="n">
-        <v>219.44</v>
+        <v>82.06</v>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Porrige</t>
+          <t>Lomo Saltado with mushrooms</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Cinnamon</t>
+          <t>Chilli pepper</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.10019</v>
+        <v>0.006690000000000001</v>
       </c>
       <c r="C46" t="n">
-        <v>0.02332</v>
+        <v>0.00261</v>
       </c>
       <c r="D46" t="n">
         <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>0.06006999999999999</v>
+        <v>3e-05</v>
       </c>
       <c r="F46" t="n">
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>0.04937999999999999</v>
+        <v>0.00522</v>
       </c>
       <c r="H46" t="n">
-        <v>0.00259</v>
+        <v>0.0018</v>
       </c>
       <c r="I46" t="n">
-        <v>0.00143</v>
+        <v>0.00492</v>
       </c>
       <c r="J46" t="n">
-        <v>0.00747</v>
+        <v>0.00123</v>
       </c>
       <c r="K46" t="n">
-        <v>0.0003</v>
+        <v>0.0004499999999999999</v>
       </c>
       <c r="L46" t="n">
-        <v>0.0002419</v>
+        <v>0.0001593</v>
       </c>
       <c r="M46" t="n">
-        <v>0.0003204</v>
+        <v>5.58e-05</v>
       </c>
       <c r="N46" t="n">
-        <v>1.72</v>
+        <v>2.49</v>
       </c>
       <c r="O46" t="n">
-        <v>54.86</v>
+        <v>118.74</v>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Porrige</t>
+          <t>Lomo Saltado with mushrooms</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Mushrooms</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>0.101465</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.039585</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.000455</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0.07916999999999999</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0.0273</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0.07462000000000001</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0.018655</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0.006825</v>
+      </c>
+      <c r="L47" t="n">
+        <v>0.00241605</v>
+      </c>
+      <c r="M47" t="n">
+        <v>0.0008463</v>
+      </c>
+      <c r="N47" t="n">
+        <v>37.765</v>
+      </c>
+      <c r="O47" t="n">
+        <v>1800.89</v>
+      </c>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with mushrooms</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Vinegar</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>0.30057</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.06995999999999999</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.18021</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0.14814</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0.007770000000000001</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0.00429</v>
+      </c>
+      <c r="J48" t="n">
+        <v>0.02241</v>
+      </c>
+      <c r="K48" t="n">
+        <v>0.0008999999999999999</v>
+      </c>
+      <c r="L48" t="n">
+        <v>0.0007257</v>
+      </c>
+      <c r="M48" t="n">
+        <v>0.0009611999999999999</v>
+      </c>
+      <c r="N48" t="n">
+        <v>5.16</v>
+      </c>
+      <c r="O48" t="n">
+        <v>164.58</v>
+      </c>
+      <c r="P48" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with mushrooms</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Soy sauce</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>0.60114</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0.13992</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.36042</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0.29628</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0.01554</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0.008580000000000001</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0.04482</v>
+      </c>
+      <c r="K49" t="n">
+        <v>0.0018</v>
+      </c>
+      <c r="L49" t="n">
+        <v>0.0014514</v>
+      </c>
+      <c r="M49" t="n">
+        <v>0.0019224</v>
+      </c>
+      <c r="N49" t="n">
+        <v>10.32</v>
+      </c>
+      <c r="O49" t="n">
+        <v>329.16</v>
+      </c>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with mushrooms</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Coriander</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>0.040076</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.009327999999999999</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.024028</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0.019752</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0.001036</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0.0005719999999999999</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0.002988</v>
+      </c>
+      <c r="K50" t="n">
+        <v>0.00012</v>
+      </c>
+      <c r="L50" t="n">
+        <v>9.676e-05</v>
+      </c>
+      <c r="M50" t="n">
+        <v>0.00012816</v>
+      </c>
+      <c r="N50" t="n">
+        <v>0.6879999999999999</v>
+      </c>
+      <c r="O50" t="n">
+        <v>21.944</v>
+      </c>
+      <c r="P50" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with mushrooms</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Garlic</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>0.150285</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.03498</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.09010499999999999</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0.07407</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0.003885</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0.002145</v>
+      </c>
+      <c r="J51" t="n">
+        <v>0.011205</v>
+      </c>
+      <c r="K51" t="n">
+        <v>0.0004499999999999999</v>
+      </c>
+      <c r="L51" t="n">
+        <v>0.00036285</v>
+      </c>
+      <c r="M51" t="n">
+        <v>0.0004806</v>
+      </c>
+      <c r="N51" t="n">
+        <v>2.58</v>
+      </c>
+      <c r="O51" t="n">
+        <v>82.29000000000001</v>
+      </c>
+      <c r="P51" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with mushrooms</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Salt</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>0.20038</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0.04664</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.12014</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0.09875999999999999</v>
+      </c>
+      <c r="H52" t="n">
+        <v>0.00518</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0.00286</v>
+      </c>
+      <c r="J52" t="n">
+        <v>0.01494</v>
+      </c>
+      <c r="K52" t="n">
+        <v>0.0005999999999999999</v>
+      </c>
+      <c r="L52" t="n">
+        <v>0.0004838</v>
+      </c>
+      <c r="M52" t="n">
+        <v>0.0006408000000000001</v>
+      </c>
+      <c r="N52" t="n">
+        <v>3.44</v>
+      </c>
+      <c r="O52" t="n">
+        <v>109.72</v>
+      </c>
+      <c r="P52" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with mushrooms</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Black pepper</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>0.40076</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0.09328</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.24028</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0.19752</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0.01036</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0.005719999999999999</v>
+      </c>
+      <c r="J53" t="n">
+        <v>0.02988</v>
+      </c>
+      <c r="K53" t="n">
+        <v>0.0012</v>
+      </c>
+      <c r="L53" t="n">
+        <v>0.0009676</v>
+      </c>
+      <c r="M53" t="n">
+        <v>0.0012816</v>
+      </c>
+      <c r="N53" t="n">
+        <v>6.88</v>
+      </c>
+      <c r="O53" t="n">
+        <v>219.44</v>
+      </c>
+      <c r="P53" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with mushrooms</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Rice</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>0.8372000000000001</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.1232</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-0.008799999999999999</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" t="n">
+        <v>1.4212</v>
+      </c>
+      <c r="H54" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0.0384</v>
+      </c>
+      <c r="J54" t="n">
+        <v>0.0336</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0.0252</v>
+      </c>
+      <c r="L54" t="n">
+        <v>0.009428000000000001</v>
+      </c>
+      <c r="M54" t="n">
+        <v>0.011888</v>
+      </c>
+      <c r="N54" t="n">
+        <v>784.8</v>
+      </c>
+      <c r="O54" t="n">
+        <v>17310</v>
+      </c>
+      <c r="P54" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with salmon</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>French fries</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>0.22659</v>
+      </c>
+      <c r="C55" t="n">
+        <v>0.06597499999999999</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-0.000455</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0.087815</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0.04277</v>
+      </c>
+      <c r="J55" t="n">
+        <v>0.020475</v>
+      </c>
+      <c r="K55" t="n">
+        <v>0.017745</v>
+      </c>
+      <c r="L55" t="n">
+        <v>0.00146965</v>
+      </c>
+      <c r="M55" t="n">
+        <v>0.00116025</v>
+      </c>
+      <c r="N55" t="n">
+        <v>19.565</v>
+      </c>
+      <c r="O55" t="n">
+        <v>922.285</v>
+      </c>
+      <c r="P55" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with salmon</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Olive oil</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>1.5021576</v>
+      </c>
+      <c r="C56" t="n">
+        <v>0.0601128</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" t="n">
+        <v>-0.0208104</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0.2358144</v>
+      </c>
+      <c r="H56" t="n">
+        <v>0.036432</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0.0266064</v>
+      </c>
+      <c r="J56" t="n">
+        <v>0.0475272</v>
+      </c>
+      <c r="K56" t="n">
+        <v>0.0025392</v>
+      </c>
+      <c r="L56" t="n">
+        <v>0.002267616</v>
+      </c>
+      <c r="M56" t="n">
+        <v>0.002221248</v>
+      </c>
+      <c r="N56" t="n">
+        <v>128.1744</v>
+      </c>
+      <c r="O56" t="n">
+        <v>10638.0888</v>
+      </c>
+      <c r="P56" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with salmon</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Tomatoes</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>0.0984</v>
+      </c>
+      <c r="C57" t="n">
+        <v>0.0546</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.1116</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0.2112</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0.0036</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0.05309999999999999</v>
+      </c>
+      <c r="J57" t="n">
+        <v>0.0435</v>
+      </c>
+      <c r="K57" t="n">
+        <v>0.0051</v>
+      </c>
+      <c r="L57" t="n">
+        <v>0.003429</v>
+      </c>
+      <c r="M57" t="n">
+        <v>0.001443</v>
+      </c>
+      <c r="N57" t="n">
+        <v>70.5</v>
+      </c>
+      <c r="O57" t="n">
+        <v>1203.9</v>
+      </c>
+      <c r="P57" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with salmon</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Onions</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>0.02409</v>
+      </c>
+      <c r="C58" t="n">
+        <v>0.007260000000000001</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0.00055</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0.02321</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0.01045</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0.00495</v>
+      </c>
+      <c r="K58" t="n">
+        <v>0.00429</v>
+      </c>
+      <c r="L58" t="n">
+        <v>0.0003344000000000001</v>
+      </c>
+      <c r="M58" t="n">
+        <v>0.000253</v>
+      </c>
+      <c r="N58" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="O58" t="n">
+        <v>82.06</v>
+      </c>
+      <c r="P58" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with salmon</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Chilli pepper</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>0.006690000000000001</v>
+      </c>
+      <c r="C59" t="n">
+        <v>0.00261</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" t="n">
+        <v>3e-05</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0.00522</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0.0018</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0.00492</v>
+      </c>
+      <c r="J59" t="n">
+        <v>0.00123</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0.0004499999999999999</v>
+      </c>
+      <c r="L59" t="n">
+        <v>0.0001593</v>
+      </c>
+      <c r="M59" t="n">
+        <v>5.58e-05</v>
+      </c>
+      <c r="N59" t="n">
+        <v>2.49</v>
+      </c>
+      <c r="O59" t="n">
+        <v>118.74</v>
+      </c>
+      <c r="P59" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with salmon</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Salmon</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>1.21485</v>
+      </c>
+      <c r="C60" t="n">
+        <v>0.32214</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.24297</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0.372645</v>
+      </c>
+      <c r="G60" t="n">
+        <v>1.63709</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0.0091</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0.050505</v>
+      </c>
+      <c r="J60" t="n">
+        <v>0.027755</v>
+      </c>
+      <c r="K60" t="n">
+        <v>0.0182</v>
+      </c>
+      <c r="L60" t="n">
+        <v>0.011375</v>
+      </c>
+      <c r="M60" t="n">
+        <v>0.04189185</v>
+      </c>
+      <c r="N60" t="n">
+        <v>598.325</v>
+      </c>
+      <c r="O60" t="n">
+        <v>6229.405</v>
+      </c>
+      <c r="P60" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with salmon</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Vinegar</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>0.30057</v>
+      </c>
+      <c r="C61" t="n">
+        <v>0.06995999999999999</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.18021</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0.14814</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0.007770000000000001</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0.00429</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0.02241</v>
+      </c>
+      <c r="K61" t="n">
+        <v>0.0008999999999999999</v>
+      </c>
+      <c r="L61" t="n">
+        <v>0.0007257</v>
+      </c>
+      <c r="M61" t="n">
+        <v>0.0009611999999999999</v>
+      </c>
+      <c r="N61" t="n">
+        <v>5.16</v>
+      </c>
+      <c r="O61" t="n">
+        <v>164.58</v>
+      </c>
+      <c r="P61" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with salmon</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Soy sauce</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>0.60114</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0.13992</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.36042</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0.29628</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0.01554</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0.008580000000000001</v>
+      </c>
+      <c r="J62" t="n">
+        <v>0.04482</v>
+      </c>
+      <c r="K62" t="n">
+        <v>0.0018</v>
+      </c>
+      <c r="L62" t="n">
+        <v>0.0014514</v>
+      </c>
+      <c r="M62" t="n">
+        <v>0.0019224</v>
+      </c>
+      <c r="N62" t="n">
+        <v>10.32</v>
+      </c>
+      <c r="O62" t="n">
+        <v>329.16</v>
+      </c>
+      <c r="P62" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with salmon</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Coriander</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>0.040076</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0.009327999999999999</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.024028</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0.019752</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0.001036</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0.0005719999999999999</v>
+      </c>
+      <c r="J63" t="n">
+        <v>0.002988</v>
+      </c>
+      <c r="K63" t="n">
+        <v>0.00012</v>
+      </c>
+      <c r="L63" t="n">
+        <v>9.676e-05</v>
+      </c>
+      <c r="M63" t="n">
+        <v>0.00012816</v>
+      </c>
+      <c r="N63" t="n">
+        <v>0.6879999999999999</v>
+      </c>
+      <c r="O63" t="n">
+        <v>21.944</v>
+      </c>
+      <c r="P63" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with salmon</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Garlic</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>0.150285</v>
+      </c>
+      <c r="C64" t="n">
+        <v>0.03498</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0.09010499999999999</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G64" t="n">
+        <v>0.07407</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0.003885</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0.002145</v>
+      </c>
+      <c r="J64" t="n">
+        <v>0.011205</v>
+      </c>
+      <c r="K64" t="n">
+        <v>0.0004499999999999999</v>
+      </c>
+      <c r="L64" t="n">
+        <v>0.00036285</v>
+      </c>
+      <c r="M64" t="n">
+        <v>0.0004806</v>
+      </c>
+      <c r="N64" t="n">
+        <v>2.58</v>
+      </c>
+      <c r="O64" t="n">
+        <v>82.29000000000001</v>
+      </c>
+      <c r="P64" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with salmon</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Salt</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>0.20038</v>
+      </c>
+      <c r="C65" t="n">
+        <v>0.04664</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0.12014</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0.09875999999999999</v>
+      </c>
+      <c r="H65" t="n">
+        <v>0.00518</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0.00286</v>
+      </c>
+      <c r="J65" t="n">
+        <v>0.01494</v>
+      </c>
+      <c r="K65" t="n">
+        <v>0.0005999999999999999</v>
+      </c>
+      <c r="L65" t="n">
+        <v>0.0004838</v>
+      </c>
+      <c r="M65" t="n">
+        <v>0.0006408000000000001</v>
+      </c>
+      <c r="N65" t="n">
+        <v>3.44</v>
+      </c>
+      <c r="O65" t="n">
+        <v>109.72</v>
+      </c>
+      <c r="P65" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with salmon</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Black pepper</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>0.40076</v>
+      </c>
+      <c r="C66" t="n">
+        <v>0.09328</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0.24028</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0</v>
+      </c>
+      <c r="G66" t="n">
+        <v>0.19752</v>
+      </c>
+      <c r="H66" t="n">
+        <v>0.01036</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0.005719999999999999</v>
+      </c>
+      <c r="J66" t="n">
+        <v>0.02988</v>
+      </c>
+      <c r="K66" t="n">
+        <v>0.0012</v>
+      </c>
+      <c r="L66" t="n">
+        <v>0.0009676</v>
+      </c>
+      <c r="M66" t="n">
+        <v>0.0012816</v>
+      </c>
+      <c r="N66" t="n">
+        <v>6.88</v>
+      </c>
+      <c r="O66" t="n">
+        <v>219.44</v>
+      </c>
+      <c r="P66" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with salmon</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Rice</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>0.8372000000000001</v>
+      </c>
+      <c r="C67" t="n">
+        <v>0.1232</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0</v>
+      </c>
+      <c r="E67" t="n">
+        <v>-0.008799999999999999</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0</v>
+      </c>
+      <c r="G67" t="n">
+        <v>1.4212</v>
+      </c>
+      <c r="H67" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="I67" t="n">
+        <v>0.0384</v>
+      </c>
+      <c r="J67" t="n">
+        <v>0.0336</v>
+      </c>
+      <c r="K67" t="n">
+        <v>0.0252</v>
+      </c>
+      <c r="L67" t="n">
+        <v>0.009428000000000001</v>
+      </c>
+      <c r="M67" t="n">
+        <v>0.011888</v>
+      </c>
+      <c r="N67" t="n">
+        <v>784.8</v>
+      </c>
+      <c r="O67" t="n">
+        <v>17310</v>
+      </c>
+      <c r="P67" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with tofu</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>French fries</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>0.22659</v>
+      </c>
+      <c r="C68" t="n">
+        <v>0.06597499999999999</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0</v>
+      </c>
+      <c r="E68" t="n">
+        <v>-0.000455</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0</v>
+      </c>
+      <c r="G68" t="n">
+        <v>0.087815</v>
+      </c>
+      <c r="H68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I68" t="n">
+        <v>0.04277</v>
+      </c>
+      <c r="J68" t="n">
+        <v>0.020475</v>
+      </c>
+      <c r="K68" t="n">
+        <v>0.017745</v>
+      </c>
+      <c r="L68" t="n">
+        <v>0.00146965</v>
+      </c>
+      <c r="M68" t="n">
+        <v>0.00116025</v>
+      </c>
+      <c r="N68" t="n">
+        <v>19.565</v>
+      </c>
+      <c r="O68" t="n">
+        <v>922.285</v>
+      </c>
+      <c r="P68" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with tofu</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Soybean Tofu</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>1.125215</v>
+      </c>
+      <c r="C69" t="n">
+        <v>0.309855</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0.43589</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0</v>
+      </c>
+      <c r="G69" t="n">
+        <v>0.225225</v>
+      </c>
+      <c r="H69" t="n">
+        <v>0.36127</v>
+      </c>
+      <c r="I69" t="n">
+        <v>0.080535</v>
+      </c>
+      <c r="J69" t="n">
+        <v>0.080535</v>
+      </c>
+      <c r="K69" t="n">
+        <v>0.12285</v>
+      </c>
+      <c r="L69" t="n">
+        <v>0.00284375</v>
+      </c>
+      <c r="M69" t="n">
+        <v>0.00251615</v>
+      </c>
+      <c r="N69" t="n">
+        <v>63.245</v>
+      </c>
+      <c r="O69" t="n">
+        <v>2177.175</v>
+      </c>
+      <c r="P69" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with tofu</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Olive oil</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>1.5021576</v>
+      </c>
+      <c r="C70" t="n">
+        <v>0.0601128</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-0.0208104</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0</v>
+      </c>
+      <c r="G70" t="n">
+        <v>0.2358144</v>
+      </c>
+      <c r="H70" t="n">
+        <v>0.036432</v>
+      </c>
+      <c r="I70" t="n">
+        <v>0.0266064</v>
+      </c>
+      <c r="J70" t="n">
+        <v>0.0475272</v>
+      </c>
+      <c r="K70" t="n">
+        <v>0.0025392</v>
+      </c>
+      <c r="L70" t="n">
+        <v>0.002267616</v>
+      </c>
+      <c r="M70" t="n">
+        <v>0.002221248</v>
+      </c>
+      <c r="N70" t="n">
+        <v>128.1744</v>
+      </c>
+      <c r="O70" t="n">
+        <v>10638.0888</v>
+      </c>
+      <c r="P70" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with tofu</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Tomatoes</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>0.0984</v>
+      </c>
+      <c r="C71" t="n">
+        <v>0.0546</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.1116</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0</v>
+      </c>
+      <c r="G71" t="n">
+        <v>0.2112</v>
+      </c>
+      <c r="H71" t="n">
+        <v>0.0036</v>
+      </c>
+      <c r="I71" t="n">
+        <v>0.05309999999999999</v>
+      </c>
+      <c r="J71" t="n">
+        <v>0.0435</v>
+      </c>
+      <c r="K71" t="n">
+        <v>0.0051</v>
+      </c>
+      <c r="L71" t="n">
+        <v>0.003429</v>
+      </c>
+      <c r="M71" t="n">
+        <v>0.001443</v>
+      </c>
+      <c r="N71" t="n">
+        <v>70.5</v>
+      </c>
+      <c r="O71" t="n">
+        <v>1203.9</v>
+      </c>
+      <c r="P71" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with tofu</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Onions</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>0.02409</v>
+      </c>
+      <c r="C72" t="n">
+        <v>0.007260000000000001</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0.00055</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0</v>
+      </c>
+      <c r="G72" t="n">
+        <v>0.02321</v>
+      </c>
+      <c r="H72" t="n">
+        <v>0</v>
+      </c>
+      <c r="I72" t="n">
+        <v>0.01045</v>
+      </c>
+      <c r="J72" t="n">
+        <v>0.00495</v>
+      </c>
+      <c r="K72" t="n">
+        <v>0.00429</v>
+      </c>
+      <c r="L72" t="n">
+        <v>0.0003344000000000001</v>
+      </c>
+      <c r="M72" t="n">
+        <v>0.000253</v>
+      </c>
+      <c r="N72" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="O72" t="n">
+        <v>82.06</v>
+      </c>
+      <c r="P72" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with tofu</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Chilli pepper</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>0.006690000000000001</v>
+      </c>
+      <c r="C73" t="n">
+        <v>0.00261</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0</v>
+      </c>
+      <c r="E73" t="n">
+        <v>3e-05</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0</v>
+      </c>
+      <c r="G73" t="n">
+        <v>0.00522</v>
+      </c>
+      <c r="H73" t="n">
+        <v>0.0018</v>
+      </c>
+      <c r="I73" t="n">
+        <v>0.00492</v>
+      </c>
+      <c r="J73" t="n">
+        <v>0.00123</v>
+      </c>
+      <c r="K73" t="n">
+        <v>0.0004499999999999999</v>
+      </c>
+      <c r="L73" t="n">
+        <v>0.0001593</v>
+      </c>
+      <c r="M73" t="n">
+        <v>5.58e-05</v>
+      </c>
+      <c r="N73" t="n">
+        <v>2.49</v>
+      </c>
+      <c r="O73" t="n">
+        <v>118.74</v>
+      </c>
+      <c r="P73" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with tofu</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Vinegar</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>0.30057</v>
+      </c>
+      <c r="C74" t="n">
+        <v>0.06995999999999999</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0.18021</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0</v>
+      </c>
+      <c r="G74" t="n">
+        <v>0.14814</v>
+      </c>
+      <c r="H74" t="n">
+        <v>0.007770000000000001</v>
+      </c>
+      <c r="I74" t="n">
+        <v>0.00429</v>
+      </c>
+      <c r="J74" t="n">
+        <v>0.02241</v>
+      </c>
+      <c r="K74" t="n">
+        <v>0.0008999999999999999</v>
+      </c>
+      <c r="L74" t="n">
+        <v>0.0007257</v>
+      </c>
+      <c r="M74" t="n">
+        <v>0.0009611999999999999</v>
+      </c>
+      <c r="N74" t="n">
+        <v>5.16</v>
+      </c>
+      <c r="O74" t="n">
+        <v>164.58</v>
+      </c>
+      <c r="P74" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with tofu</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Soy sauce</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>0.60114</v>
+      </c>
+      <c r="C75" t="n">
+        <v>0.13992</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0.36042</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0</v>
+      </c>
+      <c r="G75" t="n">
+        <v>0.29628</v>
+      </c>
+      <c r="H75" t="n">
+        <v>0.01554</v>
+      </c>
+      <c r="I75" t="n">
+        <v>0.008580000000000001</v>
+      </c>
+      <c r="J75" t="n">
+        <v>0.04482</v>
+      </c>
+      <c r="K75" t="n">
+        <v>0.0018</v>
+      </c>
+      <c r="L75" t="n">
+        <v>0.0014514</v>
+      </c>
+      <c r="M75" t="n">
+        <v>0.0019224</v>
+      </c>
+      <c r="N75" t="n">
+        <v>10.32</v>
+      </c>
+      <c r="O75" t="n">
+        <v>329.16</v>
+      </c>
+      <c r="P75" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with tofu</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Coriander</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>0.040076</v>
+      </c>
+      <c r="C76" t="n">
+        <v>0.009327999999999999</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0.024028</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G76" t="n">
+        <v>0.019752</v>
+      </c>
+      <c r="H76" t="n">
+        <v>0.001036</v>
+      </c>
+      <c r="I76" t="n">
+        <v>0.0005719999999999999</v>
+      </c>
+      <c r="J76" t="n">
+        <v>0.002988</v>
+      </c>
+      <c r="K76" t="n">
+        <v>0.00012</v>
+      </c>
+      <c r="L76" t="n">
+        <v>9.676e-05</v>
+      </c>
+      <c r="M76" t="n">
+        <v>0.00012816</v>
+      </c>
+      <c r="N76" t="n">
+        <v>0.6879999999999999</v>
+      </c>
+      <c r="O76" t="n">
+        <v>21.944</v>
+      </c>
+      <c r="P76" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with tofu</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Garlic</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>0.150285</v>
+      </c>
+      <c r="C77" t="n">
+        <v>0.03498</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.09010499999999999</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0</v>
+      </c>
+      <c r="G77" t="n">
+        <v>0.07407</v>
+      </c>
+      <c r="H77" t="n">
+        <v>0.003885</v>
+      </c>
+      <c r="I77" t="n">
+        <v>0.002145</v>
+      </c>
+      <c r="J77" t="n">
+        <v>0.011205</v>
+      </c>
+      <c r="K77" t="n">
+        <v>0.0004499999999999999</v>
+      </c>
+      <c r="L77" t="n">
+        <v>0.00036285</v>
+      </c>
+      <c r="M77" t="n">
+        <v>0.0004806</v>
+      </c>
+      <c r="N77" t="n">
+        <v>2.58</v>
+      </c>
+      <c r="O77" t="n">
+        <v>82.29000000000001</v>
+      </c>
+      <c r="P77" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with tofu</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Salt</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>0.20038</v>
+      </c>
+      <c r="C78" t="n">
+        <v>0.04664</v>
+      </c>
+      <c r="D78" t="n">
+        <v>0</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.12014</v>
+      </c>
+      <c r="F78" t="n">
+        <v>0</v>
+      </c>
+      <c r="G78" t="n">
+        <v>0.09875999999999999</v>
+      </c>
+      <c r="H78" t="n">
+        <v>0.00518</v>
+      </c>
+      <c r="I78" t="n">
+        <v>0.00286</v>
+      </c>
+      <c r="J78" t="n">
+        <v>0.01494</v>
+      </c>
+      <c r="K78" t="n">
+        <v>0.0005999999999999999</v>
+      </c>
+      <c r="L78" t="n">
+        <v>0.0004838</v>
+      </c>
+      <c r="M78" t="n">
+        <v>0.0006408000000000001</v>
+      </c>
+      <c r="N78" t="n">
+        <v>3.44</v>
+      </c>
+      <c r="O78" t="n">
+        <v>109.72</v>
+      </c>
+      <c r="P78" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with tofu</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Black pepper</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>0.40076</v>
+      </c>
+      <c r="C79" t="n">
+        <v>0.09328</v>
+      </c>
+      <c r="D79" t="n">
+        <v>0</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0.24028</v>
+      </c>
+      <c r="F79" t="n">
+        <v>0</v>
+      </c>
+      <c r="G79" t="n">
+        <v>0.19752</v>
+      </c>
+      <c r="H79" t="n">
+        <v>0.01036</v>
+      </c>
+      <c r="I79" t="n">
+        <v>0.005719999999999999</v>
+      </c>
+      <c r="J79" t="n">
+        <v>0.02988</v>
+      </c>
+      <c r="K79" t="n">
+        <v>0.0012</v>
+      </c>
+      <c r="L79" t="n">
+        <v>0.0009676</v>
+      </c>
+      <c r="M79" t="n">
+        <v>0.0012816</v>
+      </c>
+      <c r="N79" t="n">
+        <v>6.88</v>
+      </c>
+      <c r="O79" t="n">
+        <v>219.44</v>
+      </c>
+      <c r="P79" t="inlineStr">
+        <is>
+          <t>Lomo Saltado with tofu</t>
         </is>
       </c>
     </row>

</xml_diff>